<commit_message>
Added BAT temp sens
</commit_message>
<xml_diff>
--- a/Hardware/WRFL_pin_mux.xlsx
+++ b/Hardware/WRFL_pin_mux.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="15980" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="186">
   <si>
     <t>Launchpad terminal</t>
   </si>
@@ -571,13 +571,19 @@
   </si>
   <si>
     <t>BT_RESET</t>
+  </si>
+  <si>
+    <t>AIN0</t>
+  </si>
+  <si>
+    <t>BAT_TEMP_SENS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -589,6 +595,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -611,14 +633,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -950,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1176,6 +1202,15 @@
       <c r="C11" t="s">
         <v>92</v>
       </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>169</v>
+      </c>
+      <c r="F11" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
@@ -1342,13 +1377,13 @@
         <v>101</v>
       </c>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>184</v>
       </c>
       <c r="E20" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="F20" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1755,6 +1790,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
pin mux table format
</commit_message>
<xml_diff>
--- a/Hardware/WRFL_pin_mux.xlsx
+++ b/Hardware/WRFL_pin_mux.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="15980" tabRatio="500"/>
   </bookViews>
@@ -10,6 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
+  <webPublishing allowPng="1" targetScreenSize="1024x768" dpi="72" codePage="65001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="186">
   <si>
     <t>Launchpad terminal</t>
   </si>
@@ -583,7 +584,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -615,13 +616,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -633,18 +646,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -976,17 +1011,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1013,778 +1051,787 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="2" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="2" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="E29" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>110</v>
       </c>
+      <c r="E30" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="2" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="E35" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="2" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>